<commit_message>
Atualização dos notebooks para inclusão da inf de Renda Mensal
</commit_message>
<xml_diff>
--- a/Documents/Dime/DIME_ENEM_PARTICIPANTES.xlsx
+++ b/Documents/Dime/DIME_ENEM_PARTICIPANTES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estudos\SQL\Dime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoba\Documents\Enem\Documents\Dime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658053CB-031E-4A6A-9150-FD04D9C334C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BF2066-85B4-4B23-A276-0070220AB244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{3A963620-B9EE-4640-9148-C5B11AFEC753}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{3A963620-B9EE-4640-9148-C5B11AFEC753}"/>
   </bookViews>
   <sheets>
     <sheet name="DIME_FAIXA_ETARIA" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="DIME_ANO_CONCLUSAO" sheetId="7" r:id="rId8"/>
     <sheet name="DIME_ESCOLA" sheetId="8" r:id="rId9"/>
     <sheet name="DIME_ESTADO_CIVIL" sheetId="3" r:id="rId10"/>
+    <sheet name="DIME_RENDA_MENSAL" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
   <si>
     <t>Menor de 17 anos</t>
   </si>
@@ -264,6 +265,108 @@
   </si>
   <si>
     <t>Sem Referência</t>
+  </si>
+  <si>
+    <t>QUESTIONARIO_ID</t>
+  </si>
+  <si>
+    <t>QUESTIONARIO_DESCRICAO</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Nenhuma Renda</t>
+  </si>
+  <si>
+    <t>Até R$ 1.212,00</t>
+  </si>
+  <si>
+    <t>De R$ 1.212,01 até R$ 1.818,00.</t>
+  </si>
+  <si>
+    <t>De R$ 1.818,01 até R$ 2.424,00.</t>
+  </si>
+  <si>
+    <t>De R$ 2.424,01 até R$ 3.030,00.</t>
+  </si>
+  <si>
+    <t>De R$ 3.030,01 até R$ 3.636,00.</t>
+  </si>
+  <si>
+    <t>De R$ 3.636,01 até R$ 4.848,00.</t>
+  </si>
+  <si>
+    <t>De R$ 4.848,01 até R$ 6.060,00.</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>De R$ 6.060,01 até R$ 7.272,00.</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>De R$ 7.272,01 até R$ 8.484,00.</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>De R$ 8.484,01 até R$ 9.696,00.</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>De R$ 9.696,01 até R$ 10.908,00.</t>
+  </si>
+  <si>
+    <t>De R$ 10.908,01 até R$ 12.120,00.</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>De R$ 12.120,01 até R$ 14.544,00.</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>De R$ 14.544,01 até R$ 18.180,00.</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>De R$ 18.180,01 até R$ 24.240,00.</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Acima de R$ 24.240,00.</t>
   </si>
 </sst>
 </file>
@@ -884,6 +987,170 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D3C6EC-95E7-4800-A88C-1108E8E663B1}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2929C20F-D94A-4828-A868-9A9929272913}">
   <dimension ref="A1:B4"/>
@@ -1203,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76487C79-4325-4404-AF90-FDCEF11385F9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>

</xml_diff>